<commit_message>
change internal DB name
</commit_message>
<xml_diff>
--- a/Firewall-policies/Skybox_vLab_1.2.xlsx
+++ b/Firewall-policies/Skybox_vLab_1.2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E6DB04-58AC-416B-B92A-7BE3FC53392B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B1B3DD-E828-4284-8B57-5F6BAE958DA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FortiGW" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t>Source</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>LinuxWeb04</t>
+  </si>
+  <si>
+    <t>FortiDMZ</t>
   </si>
 </sst>
 </file>
@@ -419,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD0F028-4C1A-4F7C-8E95-263A98B92D2D}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +458,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -551,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed policy excel for new naming convention
</commit_message>
<xml_diff>
--- a/Firewall-policies/Skybox_vLab_1.2.xlsx
+++ b/Firewall-policies/Skybox_vLab_1.2.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B1B3DD-E828-4284-8B57-5F6BAE958DA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9EEC88-F846-4926-B924-4DBA150313FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FortiGW" sheetId="3" r:id="rId1"/>
-    <sheet name="CPMGMT" sheetId="1" r:id="rId2"/>
+    <sheet name="Fortinet_1" sheetId="3" r:id="rId1"/>
+    <sheet name="WANCPFW" sheetId="1" r:id="rId2"/>
     <sheet name="AUX" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -75,31 +75,31 @@
     <t>F</t>
   </si>
   <si>
-    <t>FortiGW</t>
-  </si>
-  <si>
-    <t>FortiWebSRV</t>
-  </si>
-  <si>
     <t>SecOps01</t>
   </si>
   <si>
     <t>SecOps02</t>
   </si>
   <si>
-    <t>Win10-C</t>
-  </si>
-  <si>
-    <t>CP-F5</t>
-  </si>
-  <si>
-    <t>Win2012-C</t>
-  </si>
-  <si>
-    <t>LinuxWeb04</t>
-  </si>
-  <si>
-    <t>FortiDMZ</t>
+    <t>Internal DB</t>
+  </si>
+  <si>
+    <t>w10c</t>
+  </si>
+  <si>
+    <t>InternalDB_1</t>
+  </si>
+  <si>
+    <t>DMZ</t>
+  </si>
+  <si>
+    <t>ws12c</t>
+  </si>
+  <si>
+    <t>webmain</t>
+  </si>
+  <si>
+    <t>Fortinet_1</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -472,10 +472,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -489,10 +489,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -506,10 +506,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +621,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -638,7 +638,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -655,7 +655,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
changing azure route table map for new naming scheme
</commit_message>
<xml_diff>
--- a/Firewall-policies/Skybox_vLab_1.2.xlsx
+++ b/Firewall-policies/Skybox_vLab_1.2.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9EEC88-F846-4926-B924-4DBA150313FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749FC2C4-49BB-4B2F-97FB-712CD76D3B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fortinet_1" sheetId="3" r:id="rId1"/>
-    <sheet name="WANCPFW" sheetId="1" r:id="rId2"/>
+    <sheet name="CPMGMT" sheetId="1" r:id="rId2"/>
     <sheet name="AUX" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -422,7 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD0F028-4C1A-4F7C-8E95-263A98B92D2D}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change name policy 1.2
</commit_message>
<xml_diff>
--- a/Firewall-policies/Skybox_vLab_1.2.xlsx
+++ b/Firewall-policies/Skybox_vLab_1.2.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D63D0FE-5159-4674-8E83-243F905492AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3702921-C6AC-4B18-A0C7-BB8CA3866016}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fortinet1" sheetId="3" r:id="rId1"/>
-    <sheet name="CPMGMT" sheetId="1" r:id="rId2"/>
+    <sheet name="Fortinet-1" sheetId="3" r:id="rId1"/>
+    <sheet name="CPMAN" sheetId="1" r:id="rId2"/>
     <sheet name="AUX" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -96,10 +96,10 @@
     <t>webmain</t>
   </si>
   <si>
-    <t>Fortinet1</t>
-  </si>
-  <si>
     <t>Internal_DB</t>
+  </si>
+  <si>
+    <t>Fortinet-1</t>
   </si>
 </sst>
 </file>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD0F028-4C1A-4F7C-8E95-263A98B92D2D}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>

</xml_diff>